<commit_message>
Přidán aktualizující-se seznam pracovišť
Netuším, jak funguje streamlit, takže snad to bude fungovat lmaooooooo
</commit_message>
<xml_diff>
--- a/results_xlsx/seminarici_bez_seminare.xlsx
+++ b/results_xlsx/seminarici_bez_seminare.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="194">
   <si>
     <t>nazev</t>
   </si>
@@ -28,16 +28,67 @@
     <t>Podnikové informační systémy</t>
   </si>
   <si>
+    <t>Fylogeneze a systém bezobratlých</t>
+  </si>
+  <si>
+    <t>Obecná botanika</t>
+  </si>
+  <si>
     <t>Fyzikální praktikum C</t>
   </si>
   <si>
     <t>Diplomový seminář</t>
   </si>
   <si>
+    <t>Souhrnný seminář a příprava k SZZ</t>
+  </si>
+  <si>
+    <t>Reg. geography of Northwestern Bohemia</t>
+  </si>
+  <si>
     <t>Regional geography of the Czech Republic</t>
   </si>
   <si>
-    <t>Reg. geography of Northwestern Bohemia</t>
+    <t>Praktické využití Petriho sítí</t>
+  </si>
+  <si>
+    <t>Informační a komunikační technologie</t>
+  </si>
+  <si>
+    <t>Semestrální projekt II</t>
+  </si>
+  <si>
+    <t>Pokročilé techniky ve VBA</t>
+  </si>
+  <si>
+    <t>Hybridní Petriho sítě</t>
+  </si>
+  <si>
+    <t>Úvod do Event-B</t>
+  </si>
+  <si>
+    <t>Programování ve VBA</t>
+  </si>
+  <si>
+    <t>Základy zpracování dat</t>
+  </si>
+  <si>
+    <t>Souborný seminář</t>
+  </si>
+  <si>
+    <t>Numerické metody</t>
+  </si>
+  <si>
+    <t>Semestrální projekt I</t>
+  </si>
+  <si>
+    <t>Manažerský excel</t>
+  </si>
+  <si>
+    <t>Základy ICT</t>
+  </si>
+  <si>
+    <t>Teorie formálních jazyků</t>
   </si>
   <si>
     <t>Počítačové modelování I</t>
@@ -46,9 +97,135 @@
     <t>Programování A</t>
   </si>
   <si>
+    <t>Teorie kódování</t>
+  </si>
+  <si>
+    <t>Aplikovaná kryptoanalýza</t>
+  </si>
+  <si>
+    <t>OLAP a Data mining</t>
+  </si>
+  <si>
+    <t>Relační databáze</t>
+  </si>
+  <si>
+    <t>Microsoft SQL Server</t>
+  </si>
+  <si>
+    <t>Matematický software</t>
+  </si>
+  <si>
+    <t>Algoritmy a datové struktury</t>
+  </si>
+  <si>
+    <t>MIS/Business Intelligence</t>
+  </si>
+  <si>
+    <t>Základy kryptologie</t>
+  </si>
+  <si>
+    <t>Úvod do zpracování a analýzy dat</t>
+  </si>
+  <si>
+    <t>Algoritmizace a programování</t>
+  </si>
+  <si>
+    <t>Praktikum z databázových systémů</t>
+  </si>
+  <si>
+    <t>Seminář k diplomové práci A</t>
+  </si>
+  <si>
+    <t>Odborný seminář A</t>
+  </si>
+  <si>
+    <t>Organické syntézy</t>
+  </si>
+  <si>
+    <t>Seminář k diplomové práci B</t>
+  </si>
+  <si>
+    <t>Odborný seminář B</t>
+  </si>
+  <si>
+    <t>Odborná angličtina</t>
+  </si>
+  <si>
+    <t>Odborný seminář IT</t>
+  </si>
+  <si>
+    <t>Mezioborové souvislosti</t>
+  </si>
+  <si>
+    <t>Projektový seminář</t>
+  </si>
+  <si>
+    <t>Právní a ekonomické minimum pro IT</t>
+  </si>
+  <si>
+    <t>Projektový seminář I</t>
+  </si>
+  <si>
+    <t>Základy ekonomie</t>
+  </si>
+  <si>
+    <t>Projektový seminář II</t>
+  </si>
+  <si>
+    <t>Projektový seminář III</t>
+  </si>
+  <si>
+    <t>Odborná prezentace</t>
+  </si>
+  <si>
+    <t>Semestrální projekt III</t>
+  </si>
+  <si>
+    <t>Úvod do kombinovaného studia</t>
+  </si>
+  <si>
+    <t>Základy ekonomie a managementu</t>
+  </si>
+  <si>
+    <t>Analýza a vizualizace podnikových dat II</t>
+  </si>
+  <si>
+    <t>Projektové výzvy a strategie v IT</t>
+  </si>
+  <si>
+    <t>Aplikace výpočetní geometrie</t>
+  </si>
+  <si>
+    <t>Úvod od jazyka R</t>
+  </si>
+  <si>
+    <t>Odborná praxe</t>
+  </si>
+  <si>
+    <t>Prezentace projektu</t>
+  </si>
+  <si>
+    <t>Projektový seminář IV</t>
+  </si>
+  <si>
+    <t>Dependabilita SW a HW systémů</t>
+  </si>
+  <si>
+    <t>Dependabilita informačních systémů</t>
+  </si>
+  <si>
+    <t>Softwarové inženýrství</t>
+  </si>
+  <si>
+    <t>Značkovací jazyky</t>
+  </si>
+  <si>
     <t>Identif. a hodn. ekosystémových služeb</t>
   </si>
   <si>
+    <t>Marketing</t>
+  </si>
+  <si>
     <t>Sociální sítě</t>
   </si>
   <si>
@@ -67,16 +244,19 @@
     <t>Letní geografická škola</t>
   </si>
   <si>
+    <t>Praktikum počítačového modelování I</t>
+  </si>
+  <si>
+    <t>Praktikum počítačového modelování II</t>
+  </si>
+  <si>
     <t>Reflektivní seminář pedagogické praxe</t>
   </si>
   <si>
-    <t>Softwarové inženýrství</t>
-  </si>
-  <si>
     <t>Introduction to MATLAB</t>
   </si>
   <si>
-    <t>Odborná prezentace</t>
+    <t>Optimální rozhodování</t>
   </si>
   <si>
     <t>EIS</t>
@@ -85,30 +265,294 @@
     <t>KEIS</t>
   </si>
   <si>
+    <t>P302</t>
+  </si>
+  <si>
+    <t>P112</t>
+  </si>
+  <si>
     <t>K521</t>
   </si>
   <si>
     <t>K505</t>
   </si>
   <si>
+    <t>M403</t>
+  </si>
+  <si>
+    <t>E100</t>
+  </si>
+  <si>
     <t>E101</t>
   </si>
   <si>
-    <t>E100</t>
+    <t>PVPS</t>
+  </si>
+  <si>
+    <t>ICT</t>
+  </si>
+  <si>
+    <t>KSP2</t>
+  </si>
+  <si>
+    <t>0169</t>
+  </si>
+  <si>
+    <t>0168</t>
+  </si>
+  <si>
+    <t>0175</t>
+  </si>
+  <si>
+    <t>0054</t>
+  </si>
+  <si>
+    <t>SP2</t>
+  </si>
+  <si>
+    <t>ZZD</t>
+  </si>
+  <si>
+    <t>KPVPS</t>
+  </si>
+  <si>
+    <t>KZZD</t>
+  </si>
+  <si>
+    <t>0185</t>
+  </si>
+  <si>
+    <t>KNUM</t>
+  </si>
+  <si>
+    <t>KSP1</t>
+  </si>
+  <si>
+    <t>0131</t>
+  </si>
+  <si>
+    <t>ZICT</t>
+  </si>
+  <si>
+    <t>TFL</t>
+  </si>
+  <si>
+    <t>NUM</t>
   </si>
   <si>
     <t>K107</t>
   </si>
   <si>
+    <t>K103</t>
+  </si>
+  <si>
     <t>P107</t>
   </si>
   <si>
-    <t>K103</t>
+    <t>TKO</t>
+  </si>
+  <si>
+    <t>AKA</t>
+  </si>
+  <si>
+    <t>KICT</t>
+  </si>
+  <si>
+    <t>ODM</t>
+  </si>
+  <si>
+    <t>KZICT</t>
+  </si>
+  <si>
+    <t>YRDB</t>
+  </si>
+  <si>
+    <t>0204</t>
+  </si>
+  <si>
+    <t>KMSW</t>
+  </si>
+  <si>
+    <t>XADS</t>
+  </si>
+  <si>
+    <t>0152</t>
+  </si>
+  <si>
+    <t>KZKR</t>
+  </si>
+  <si>
+    <t>MSW</t>
+  </si>
+  <si>
+    <t>0167</t>
+  </si>
+  <si>
+    <t>KAKA</t>
+  </si>
+  <si>
+    <t>YAPR</t>
+  </si>
+  <si>
+    <t>PDSY</t>
+  </si>
+  <si>
+    <t>KODM</t>
+  </si>
+  <si>
+    <t>N231</t>
+  </si>
+  <si>
+    <t>BK214</t>
+  </si>
+  <si>
+    <t>PD09</t>
+  </si>
+  <si>
+    <t>N326</t>
+  </si>
+  <si>
+    <t>BK308</t>
+  </si>
+  <si>
+    <t>KN231</t>
+  </si>
+  <si>
+    <t>BK213</t>
+  </si>
+  <si>
+    <t>B213</t>
+  </si>
+  <si>
+    <t>KN326</t>
+  </si>
+  <si>
+    <t>B214</t>
+  </si>
+  <si>
+    <t>B308</t>
+  </si>
+  <si>
+    <t>OSIT</t>
+  </si>
+  <si>
+    <t>MES</t>
+  </si>
+  <si>
+    <t>KMES</t>
+  </si>
+  <si>
+    <t>KPROJ</t>
+  </si>
+  <si>
+    <t>KPEM</t>
+  </si>
+  <si>
+    <t>PS1</t>
+  </si>
+  <si>
+    <t>ZEK</t>
+  </si>
+  <si>
+    <t>PS2</t>
+  </si>
+  <si>
+    <t>PS3</t>
+  </si>
+  <si>
+    <t>OPRE</t>
+  </si>
+  <si>
+    <t>SP3</t>
+  </si>
+  <si>
+    <t>KPS1</t>
+  </si>
+  <si>
+    <t>KUKS</t>
+  </si>
+  <si>
+    <t>KZEK</t>
+  </si>
+  <si>
+    <t>PROJ</t>
+  </si>
+  <si>
+    <t>ZEM</t>
+  </si>
+  <si>
+    <t>AVD2</t>
+  </si>
+  <si>
+    <t>PVS</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>PEM</t>
+  </si>
+  <si>
+    <t>UDR</t>
+  </si>
+  <si>
+    <t>KAVG</t>
+  </si>
+  <si>
+    <t>KPS2</t>
+  </si>
+  <si>
+    <t>KPVS</t>
+  </si>
+  <si>
+    <t>SP1</t>
+  </si>
+  <si>
+    <t>PRAX</t>
+  </si>
+  <si>
+    <t>PREP</t>
+  </si>
+  <si>
+    <t>KAVD2</t>
+  </si>
+  <si>
+    <t>KOPRE</t>
+  </si>
+  <si>
+    <t>KSP3</t>
+  </si>
+  <si>
+    <t>PS4</t>
+  </si>
+  <si>
+    <t>KDSHS</t>
+  </si>
+  <si>
+    <t>KDIS</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>SWI</t>
+  </si>
+  <si>
+    <t>KSWI</t>
+  </si>
+  <si>
+    <t>MRL</t>
+  </si>
+  <si>
+    <t>DSHS</t>
   </si>
   <si>
     <t>0153</t>
   </si>
   <si>
+    <t>MARK</t>
+  </si>
+  <si>
     <t>SON</t>
   </si>
   <si>
@@ -127,28 +571,31 @@
     <t>0158</t>
   </si>
   <si>
+    <t>M103</t>
+  </si>
+  <si>
+    <t>M203</t>
+  </si>
+  <si>
+    <t>KSPP</t>
+  </si>
+  <si>
     <t>KRSPP</t>
   </si>
   <si>
-    <t>KSPP</t>
-  </si>
-  <si>
     <t>RSPP</t>
   </si>
   <si>
-    <t>SWI</t>
-  </si>
-  <si>
-    <t>KSWI</t>
-  </si>
-  <si>
     <t>ITM</t>
   </si>
   <si>
-    <t>KOPRE</t>
-  </si>
-  <si>
-    <t>OPRE</t>
+    <t>OAN</t>
+  </si>
+  <si>
+    <t>KOPR</t>
+  </si>
+  <si>
+    <t>KOAN</t>
   </si>
 </sst>
 </file>
@@ -210,8 +657,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:C34" totalsRowShown="0">
-  <autoFilter ref="A1:C34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:C147" totalsRowShown="0">
+  <autoFilter ref="A1:C147"/>
   <tableColumns count="3">
     <tableColumn id="1" name="nazev" dataDxfId="0"/>
     <tableColumn id="2" name="zkratka" dataDxfId="0"/>
@@ -506,7 +953,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -528,7 +975,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="C2" s="2">
         <v>14</v>
@@ -539,7 +986,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2">
         <v>14</v>
@@ -550,10 +997,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="C4" s="2">
-        <v>302</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -561,10 +1008,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="C5" s="2">
-        <v>306</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -572,10 +1019,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="C6" s="2">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -583,10 +1030,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C7" s="2">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -594,296 +1041,1539 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="C8" s="2">
-        <v>612</v>
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="C9" s="2">
-        <v>612</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="C10" s="2">
-        <v>612</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="C11" s="2">
-        <v>1609</v>
+        <v>449</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="C12" s="2">
-        <v>1609</v>
+        <v>449</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="C13" s="2">
-        <v>2527</v>
+        <v>449</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
       <c r="C14" s="2">
-        <v>3457</v>
+        <v>449</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="C15" s="2">
-        <v>3457</v>
+        <v>449</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="C16" s="2">
-        <v>3606</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="C17" s="2">
-        <v>3606</v>
+        <v>449</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="C18" s="2">
-        <v>4190</v>
+        <v>449</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
       <c r="C19" s="2">
-        <v>4221</v>
+        <v>449</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="C20" s="2">
-        <v>4625</v>
+        <v>449</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="C21" s="2">
-        <v>4746</v>
+        <v>449</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
       <c r="C22" s="2">
-        <v>4746</v>
+        <v>449</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="C23" s="2">
-        <v>4747</v>
+        <v>449</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="C24" s="2">
-        <v>4991</v>
+        <v>449</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="C25" s="2">
-        <v>4991</v>
+        <v>449</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="C26" s="2">
-        <v>5886</v>
+        <v>449</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="C27" s="2">
-        <v>8021</v>
+        <v>449</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="C28" s="2">
-        <v>8021</v>
+        <v>449</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="C29" s="2">
-        <v>8021</v>
+        <v>612</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
       <c r="C30" s="2">
-        <v>8093</v>
+        <v>612</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
       <c r="C31" s="2">
-        <v>8093</v>
+        <v>612</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="C32" s="2">
-        <v>8514</v>
+        <v>835</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="C33" s="2">
-        <v>8514</v>
+        <v>835</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C47" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C49" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="2">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" s="2">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C54" s="2">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" s="2">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C56" s="2">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" s="2">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C58" s="2">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C59" s="2">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C60" s="2">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C61" s="2">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C62" s="2">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C63" s="2">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C64" s="2">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C65" s="2">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C66" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C67" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C68" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C69" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C70" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C71" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C72" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C73" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C75" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C76" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C77" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C78" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C79" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C80" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C81" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C82" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C83" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C84" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C85" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C86" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C87" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C88" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C89" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C90" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C91" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C92" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C93" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B94" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C94" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C95" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C96" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C97" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C98" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C99" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C100" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C101" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C102" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C103" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C104" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C105" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C106" s="2">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C107" s="2">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C108" s="2">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C109" s="2">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C110" s="2">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C111" s="2">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C112" s="2">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C113" s="2">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C114" s="2">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C115" s="2">
+        <v>2527</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C116" s="2">
+        <v>3143</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C117" s="2">
+        <v>3457</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C118" s="2">
+        <v>3457</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C119" s="2">
+        <v>3606</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C120" s="2">
+        <v>3606</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C121" s="2">
+        <v>4190</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C122" s="2">
+        <v>4221</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C123" s="2">
+        <v>4625</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C124" s="2">
+        <v>4746</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C125" s="2">
+        <v>4746</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C126" s="2">
+        <v>4747</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C127" s="2">
+        <v>4991</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C128" s="2">
+        <v>4991</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C129" s="2">
+        <v>5886</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C130" s="2">
+        <v>5958</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C131" s="2">
+        <v>5958</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C132" s="2">
+        <v>8021</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C133" s="2">
+        <v>8021</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C134" s="2">
+        <v>8021</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C135" s="2">
+        <v>8093</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C136" s="2">
+        <v>8093</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C137" s="2">
+        <v>8514</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C138" s="2">
+        <v>8514</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C139" s="2">
+        <v>8514</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="2">
-        <v>8514</v>
+      <c r="B140" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C140" s="2">
+        <v>9114</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C141" s="2">
+        <v>9114</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C142" s="2">
+        <v>9114</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C143" s="2">
+        <v>9114</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C144" s="2">
+        <v>9114</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C145" s="2">
+        <v>9114</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C146" s="2">
+        <v>9303</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C147" s="2">
+        <v>9303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>